<commit_message>
Added ground truth and new ENU method/data
</commit_message>
<xml_diff>
--- a/Data/IMUReadingsClip/DefenderCorner1aInside.xlsx
+++ b/Data/IMUReadingsClip/DefenderCorner1aInside.xlsx
@@ -15,7 +15,55 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+  <si>
+    <t>utcTimeMillis</t>
+  </si>
+  <si>
+    <t>elapsedRealtimeNanos</t>
+  </si>
+  <si>
+    <t>UncalAccelXMps2</t>
+  </si>
+  <si>
+    <t>UncalAccelYMps2</t>
+  </si>
+  <si>
+    <t>UncalAccelZMps2</t>
+  </si>
+  <si>
+    <t>BiasXMps2</t>
+  </si>
+  <si>
+    <t>BiasYMps2</t>
+  </si>
+  <si>
+    <t>BiasZMps2</t>
+  </si>
+  <si>
+    <t>CalAccelXMps2</t>
+  </si>
+  <si>
+    <t>CalAccelYMps2</t>
+  </si>
+  <si>
+    <t>CalAccelZMps2</t>
+  </si>
+  <si>
+    <t>utcTimeMillis</t>
+  </si>
+  <si>
+    <t>elapsedRealtimeNanos</t>
+  </si>
+  <si>
+    <t>yawDeg</t>
+  </si>
+  <si>
+    <t>rollDeg</t>
+  </si>
+  <si>
+    <t>pitchDeg</t>
+  </si>
   <si>
     <t>utcTimeMillis</t>
   </si>
@@ -83,7 +131,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -93,14 +141,18 @@
     </border>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -128,37 +180,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2">
@@ -22719,19 +22771,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2">

</xml_diff>